<commit_message>
latest changes - 6-jun-2018
</commit_message>
<xml_diff>
--- a/src/test/java/com/test/automation/uiAutomation/Data/TestSuite1.xlsx
+++ b/src/test/java/com/test/automation/uiAutomation/Data/TestSuite1.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20040" windowHeight="6225" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19695" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TC01" sheetId="3" r:id="rId2"/>
-    <sheet name="TC02" sheetId="7" r:id="rId3"/>
+    <sheet name="TC02" sheetId="9" r:id="rId3"/>
     <sheet name="TC03" sheetId="8" r:id="rId4"/>
+    <sheet name="TC04" sheetId="11" r:id="rId5"/>
+    <sheet name="TC05" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="185">
   <si>
     <t>TCID</t>
   </si>
@@ -168,247 +170,418 @@
     <t>TS12</t>
   </si>
   <si>
+    <t>Click on Engagement menu</t>
+  </si>
+  <si>
+    <t>Verify calls menu</t>
+  </si>
+  <si>
+    <t>CallsMenu</t>
+  </si>
+  <si>
+    <t>HomeMenu</t>
+  </si>
+  <si>
+    <t>EngagementMenu</t>
+  </si>
+  <si>
+    <t>PerformanceMenu</t>
+  </si>
+  <si>
+    <t>FinancialsMenu</t>
+  </si>
+  <si>
+    <t>TopMenuIcon</t>
+  </si>
+  <si>
+    <t>LogoffLink</t>
+  </si>
+  <si>
+    <t>TS13</t>
+  </si>
+  <si>
+    <t>PatientsMenu</t>
+  </si>
+  <si>
+    <t>Verify patients menu</t>
+  </si>
+  <si>
+    <t>AppointmentsMenu</t>
+  </si>
+  <si>
+    <t>Verify appointments menu</t>
+  </si>
+  <si>
+    <t>TS14</t>
+  </si>
+  <si>
+    <t>Click on performance menu</t>
+  </si>
+  <si>
+    <t>CheckInMenu</t>
+  </si>
+  <si>
+    <t>ClinicalTimeMenu</t>
+  </si>
+  <si>
+    <t>CheckoutMenu</t>
+  </si>
+  <si>
+    <t>PrescriptionMenu</t>
+  </si>
+  <si>
+    <t>MarketingMenu</t>
+  </si>
+  <si>
+    <t>TS15</t>
+  </si>
+  <si>
+    <t>Verify checkin menu</t>
+  </si>
+  <si>
+    <t>Verify clinicaltime menu</t>
+  </si>
+  <si>
+    <t>Verify checkout menu</t>
+  </si>
+  <si>
+    <t>Verify prescription menu</t>
+  </si>
+  <si>
+    <t>Verify marketing menu</t>
+  </si>
+  <si>
+    <t>TS16</t>
+  </si>
+  <si>
+    <t>TS17</t>
+  </si>
+  <si>
+    <t>TS18</t>
+  </si>
+  <si>
+    <t>TS19</t>
+  </si>
+  <si>
+    <t>TS20</t>
+  </si>
+  <si>
+    <t>Click on financials menu</t>
+  </si>
+  <si>
+    <t>TS21</t>
+  </si>
+  <si>
+    <t>BillingMenu</t>
+  </si>
+  <si>
+    <t>ClaimRejectionMenu</t>
+  </si>
+  <si>
+    <t>ReceivalblesMenu</t>
+  </si>
+  <si>
+    <t>ARMenu</t>
+  </si>
+  <si>
+    <t>DenialsMenu</t>
+  </si>
+  <si>
+    <t>WriteoffsMenu</t>
+  </si>
+  <si>
+    <t>PayerAnalysisMenu</t>
+  </si>
+  <si>
+    <t>CustomMenu</t>
+  </si>
+  <si>
+    <t>Verify billing menu</t>
+  </si>
+  <si>
+    <t>Verify claim rejections menu</t>
+  </si>
+  <si>
+    <t>Verify receivables menu</t>
+  </si>
+  <si>
+    <t>Verify AR menu</t>
+  </si>
+  <si>
+    <t>Verify Denials menu</t>
+  </si>
+  <si>
+    <t>Verify writeoffs menu</t>
+  </si>
+  <si>
+    <t>Verify payer analysis menu</t>
+  </si>
+  <si>
+    <t>Verify custom menu</t>
+  </si>
+  <si>
+    <t>TS22</t>
+  </si>
+  <si>
+    <t>TS23</t>
+  </si>
+  <si>
+    <t>TS24</t>
+  </si>
+  <si>
+    <t>TS25</t>
+  </si>
+  <si>
+    <t>TS26</t>
+  </si>
+  <si>
+    <t>TS27</t>
+  </si>
+  <si>
+    <t>TS28</t>
+  </si>
+  <si>
+    <t>TS29</t>
+  </si>
+  <si>
+    <t>TS30</t>
+  </si>
+  <si>
+    <t>TS31</t>
+  </si>
+  <si>
+    <t>TS32</t>
+  </si>
+  <si>
+    <t>TS33</t>
+  </si>
+  <si>
+    <t>TS34</t>
+  </si>
+  <si>
+    <t>TS35</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>VerifyCPAwidget</t>
+  </si>
+  <si>
+    <t>Verify widget title</t>
+  </si>
+  <si>
+    <t>CPATitle</t>
+  </si>
+  <si>
+    <t>HoverOn</t>
+  </si>
+  <si>
+    <t>Hover on info icon</t>
+  </si>
+  <si>
+    <t>CPAInfoIcon</t>
+  </si>
+  <si>
+    <t>CPAInfoText</t>
+  </si>
+  <si>
+    <t>Verify widget Info Text</t>
+  </si>
+  <si>
+    <t>Click on receivables menu</t>
+  </si>
+  <si>
+    <t>expliciteWait</t>
+  </si>
+  <si>
+    <t>Waiting for Financials menu</t>
+  </si>
+  <si>
+    <t>Waiting for payments menu</t>
+  </si>
+  <si>
+    <t>Waiting for CPA title</t>
+  </si>
+  <si>
+    <t>Waiting for CPA info text</t>
+  </si>
+  <si>
+    <t>Verify user name text box</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>https://wshcloud.com/</t>
-  </si>
-  <si>
-    <t>Click on Engagement menu</t>
-  </si>
-  <si>
-    <t>Verify calls menu</t>
-  </si>
-  <si>
-    <t>CallsMenu</t>
-  </si>
-  <si>
-    <t>HomeMenu</t>
-  </si>
-  <si>
-    <t>EngagementMenu</t>
-  </si>
-  <si>
-    <t>PerformanceMenu</t>
-  </si>
-  <si>
-    <t>FinancialsMenu</t>
-  </si>
-  <si>
-    <t>TopMenuIcon</t>
-  </si>
-  <si>
-    <t>LogoffLink</t>
-  </si>
-  <si>
-    <t>TS13</t>
-  </si>
-  <si>
-    <t>PatientsMenu</t>
-  </si>
-  <si>
-    <t>Verify patients menu</t>
-  </si>
-  <si>
-    <t>AppointmentsMenu</t>
-  </si>
-  <si>
-    <t>Verify appointments menu</t>
-  </si>
-  <si>
-    <t>TS14</t>
-  </si>
-  <si>
-    <t>Click on performance menu</t>
-  </si>
-  <si>
-    <t>CheckInMenu</t>
-  </si>
-  <si>
-    <t>ClinicalTimeMenu</t>
-  </si>
-  <si>
-    <t>CheckoutMenu</t>
-  </si>
-  <si>
-    <t>PrescriptionMenu</t>
-  </si>
-  <si>
-    <t>MarketingMenu</t>
-  </si>
-  <si>
-    <t>TS15</t>
-  </si>
-  <si>
-    <t>Verify checkin menu</t>
-  </si>
-  <si>
-    <t>Verify clinicaltime menu</t>
-  </si>
-  <si>
-    <t>Verify checkout menu</t>
-  </si>
-  <si>
-    <t>Verify prescription menu</t>
-  </si>
-  <si>
-    <t>Verify marketing menu</t>
-  </si>
-  <si>
-    <t>TS16</t>
-  </si>
-  <si>
-    <t>TS17</t>
-  </si>
-  <si>
-    <t>TS18</t>
-  </si>
-  <si>
-    <t>TS19</t>
-  </si>
-  <si>
-    <t>TS20</t>
-  </si>
-  <si>
-    <t>Click on financials menu</t>
-  </si>
-  <si>
-    <t>TS21</t>
-  </si>
-  <si>
-    <t>BillingMenu</t>
-  </si>
-  <si>
-    <t>ClaimRejectionMenu</t>
-  </si>
-  <si>
-    <t>ReceivalblesMenu</t>
-  </si>
-  <si>
-    <t>ARMenu</t>
-  </si>
-  <si>
-    <t>DenialsMenu</t>
-  </si>
-  <si>
-    <t>WriteoffsMenu</t>
-  </si>
-  <si>
-    <t>PayerAnalysisMenu</t>
-  </si>
-  <si>
-    <t>CustomMenu</t>
-  </si>
-  <si>
-    <t>Verify billing menu</t>
-  </si>
-  <si>
-    <t>Verify claim rejections menu</t>
-  </si>
-  <si>
-    <t>Verify receivables menu</t>
-  </si>
-  <si>
-    <t>Verify AR menu</t>
-  </si>
-  <si>
-    <t>Verify Denials menu</t>
-  </si>
-  <si>
-    <t>Verify writeoffs menu</t>
-  </si>
-  <si>
-    <t>Verify payer analysis menu</t>
-  </si>
-  <si>
-    <t>Verify custom menu</t>
-  </si>
-  <si>
-    <t>TS22</t>
-  </si>
-  <si>
-    <t>TS23</t>
-  </si>
-  <si>
-    <t>TS24</t>
-  </si>
-  <si>
-    <t>TS25</t>
-  </si>
-  <si>
-    <t>TS26</t>
-  </si>
-  <si>
-    <t>TS27</t>
-  </si>
-  <si>
-    <t>TS28</t>
-  </si>
-  <si>
-    <t>TS29</t>
-  </si>
-  <si>
-    <t>TS30</t>
-  </si>
-  <si>
-    <t>TS31</t>
-  </si>
-  <si>
-    <t>TS32</t>
-  </si>
-  <si>
-    <t>TS33</t>
-  </si>
-  <si>
-    <t>TS34</t>
-  </si>
-  <si>
-    <t>TS35</t>
-  </si>
-  <si>
-    <t>TC03</t>
-  </si>
-  <si>
-    <t>VerifyCPAwidget</t>
-  </si>
-  <si>
-    <t>Verify widget title</t>
-  </si>
-  <si>
-    <t>CPATitle</t>
-  </si>
-  <si>
-    <t>HoverOn</t>
-  </si>
-  <si>
-    <t>Hover on info icon</t>
-  </si>
-  <si>
-    <t>CPAInfoIcon</t>
-  </si>
-  <si>
-    <t>CPAInfoText</t>
-  </si>
-  <si>
-    <t>Verify widget Info Text</t>
-  </si>
-  <si>
-    <t>Click on receivables menu</t>
-  </si>
-  <si>
-    <t>expliciteWait</t>
-  </si>
-  <si>
-    <t>Waiting for Financials menu</t>
-  </si>
-  <si>
-    <t>Waiting for payments menu</t>
-  </si>
-  <si>
-    <t>Waiting for CPA title</t>
-  </si>
-  <si>
-    <t>Waiting for CPA info text</t>
+    <t>VerifyBillingVolumewidgetTitlesandInfotext</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>BillingStatusTitle</t>
+  </si>
+  <si>
+    <t>Waiting for Billing status title</t>
+  </si>
+  <si>
+    <t>Verify Billing status title</t>
+  </si>
+  <si>
+    <t>BillingStatusInfoText</t>
+  </si>
+  <si>
+    <t>BillingStatusInfoIcon</t>
+  </si>
+  <si>
+    <t>Waiting for Billing status info text</t>
+  </si>
+  <si>
+    <t>Verify Billing status widget Info Text</t>
+  </si>
+  <si>
+    <t>Waiting for billing volume menu</t>
+  </si>
+  <si>
+    <t>Click on billing volume menu</t>
+  </si>
+  <si>
+    <t>Waiting for Daily visits vs bills created title</t>
+  </si>
+  <si>
+    <t>DailyVisitsBillsTitle</t>
+  </si>
+  <si>
+    <t>DailyVisitsBillsInfoText</t>
+  </si>
+  <si>
+    <t>DailyVisitsBillsInfoIcon</t>
+  </si>
+  <si>
+    <t>Verify Daily visits vs bills created title</t>
+  </si>
+  <si>
+    <t>Waiting for Daily visits vs bills created info text</t>
+  </si>
+  <si>
+    <t>Verify Daily visits vs bills created widget Info Text</t>
+  </si>
+  <si>
+    <t>BillSubmissionTitle</t>
+  </si>
+  <si>
+    <t>BillSubmissionInfoIcon</t>
+  </si>
+  <si>
+    <t>BillSubmissionInfoText</t>
+  </si>
+  <si>
+    <t>Waiting for Daily Billing back log title</t>
+  </si>
+  <si>
+    <t>Verify Daily Billing back log title</t>
+  </si>
+  <si>
+    <t>Waiting for Daily Billing back log info text</t>
+  </si>
+  <si>
+    <t>Verify Daily Billing back log widget Info Text</t>
+  </si>
+  <si>
+    <t>BillingBacklogTitle</t>
+  </si>
+  <si>
+    <t>BillingBacklogInfoIcon</t>
+  </si>
+  <si>
+    <t>BillingBacklogInfoText</t>
+  </si>
+  <si>
+    <t>DailyUnsignedTitle</t>
+  </si>
+  <si>
+    <t>DailyUnsignedInfoText</t>
+  </si>
+  <si>
+    <t>DailyUnsignedInfoIcon</t>
+  </si>
+  <si>
+    <t>Waiting for Daily unsigned title</t>
+  </si>
+  <si>
+    <t>Verify Daily unsigned title</t>
+  </si>
+  <si>
+    <t>Waiting for Daily unsigned info text</t>
+  </si>
+  <si>
+    <t>TS36</t>
+  </si>
+  <si>
+    <t>TS37</t>
+  </si>
+  <si>
+    <t>Verify Daily unsigned widget Info Text</t>
+  </si>
+  <si>
+    <t>Waiting for Bill &amp; submission lag info text</t>
+  </si>
+  <si>
+    <t>VerifyBill&amp; submission lag Info Text</t>
+  </si>
+  <si>
+    <t>Verify Bill &amp; submission lag title</t>
+  </si>
+  <si>
+    <t>Waiting for Bill &amp; submission lag  title</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>TS38</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>AddToHomePage</t>
+  </si>
+  <si>
+    <t>Waiting for Daily visits vs bills created title Menu</t>
+  </si>
+  <si>
+    <t>DailyVisitsBillsTitleMenu</t>
+  </si>
+  <si>
+    <t>DailyVisitsBillsAddToHome</t>
+  </si>
+  <si>
+    <t>Wating for add to home page link</t>
+  </si>
+  <si>
+    <t>Click on Add to home page link</t>
+  </si>
+  <si>
+    <t>Click on home tab</t>
+  </si>
+  <si>
+    <t>Click on  Daily visits vs bills created title menu</t>
+  </si>
+  <si>
+    <t>Click on Remove from page link</t>
+  </si>
+  <si>
+    <t>Wait for remove page from link</t>
+  </si>
+  <si>
+    <t>https://test.wshcloud.com/</t>
+  </si>
+  <si>
+    <t>Homepage_DailyVisitsBillsTitleMenu</t>
+  </si>
+  <si>
+    <t>Homepage_DailyVisitsBillsRemoveWidget</t>
   </si>
 </sst>
 </file>
@@ -786,15 +959,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -816,7 +989,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -827,18 +1000,40 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -848,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -895,7 +1090,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -910,14 +1105,15 @@
         <v>24</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -985,14 +1181,15 @@
         <v>24</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -1005,7 +1202,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -1019,14 +1216,15 @@
         <v>24</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -1039,7 +1237,27 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1055,14 +1273,14 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:F36"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1097,7 +1315,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -1112,14 +1330,15 @@
         <v>24</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -1187,14 +1406,15 @@
         <v>24</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -1207,13 +1427,13 @@
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1227,13 +1447,13 @@
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1247,13 +1467,13 @@
         <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1267,13 +1487,13 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1281,13 +1501,13 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
@@ -1302,67 +1522,68 @@
         <v>24</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -1371,153 +1592,154 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
@@ -1526,184 +1748,185 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
         <v>39</v>
@@ -1712,7 +1935,7 @@
         <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
@@ -1720,24 +1943,25 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="D35" t="s">
+        <v>55</v>
       </c>
       <c r="E35" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B36" t="s">
         <v>40</v>
@@ -1746,7 +1970,10 @@
         <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1759,19 +1986,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1805,7 +2032,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -1892,13 +2119,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -1910,13 +2137,13 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -1927,13 +2154,13 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -1944,13 +2171,13 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -1961,13 +2188,13 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -1978,19 +2205,19 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1998,13 +2225,13 @@
         <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
@@ -2012,16 +2239,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
@@ -2029,27 +2256,1148 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>153</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" t="s">
+        <v>157</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>162</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" t="s">
+        <v>184</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>68</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
@@ -2058,7 +3406,7 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -2066,16 +3414,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
@@ -2084,7 +3432,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
@@ -2093,7 +3441,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>

</xml_diff>